<commit_message>
Ajuste recurso aprovechado escaleta mat 7 tema 14
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion14/Escaleta_MA_07_14_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion14/Escaleta_MA_07_14_CO.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="238">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1017,6 +1017,9 @@
   </si>
   <si>
     <t>Actividad para practicar la medidas de tendencia central y las tablas de frecuencia</t>
+  </si>
+  <si>
+    <t>Practica los distintos parámetros estadísticos</t>
   </si>
 </sst>
 </file>
@@ -1531,7 +1534,35 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1571,34 +1602,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1907,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR1090"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C22"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1942,94 +1945,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="97" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="82" t="s">
+      <c r="G1" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="H1" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="91" t="s">
+      <c r="I1" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="82" t="s">
+      <c r="L1" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="85" t="s">
+      <c r="M1" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="85"/>
-      <c r="O1" s="79" t="s">
+      <c r="N1" s="95"/>
+      <c r="O1" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="P1" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="Q1" s="93" t="s">
+      <c r="Q1" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="97" t="s">
+      <c r="R1" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="93" t="s">
+      <c r="S1" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="95" t="s">
+      <c r="T1" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="93" t="s">
+      <c r="U1" s="84" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:44" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="82"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="92"/>
       <c r="M2" s="44" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="98"/>
-      <c r="S2" s="94"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="94"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="89"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="85"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -3129,46 +3132,46 @@
       <c r="C20" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="99" t="s">
+      <c r="D20" s="79" t="s">
         <v>233</v>
       </c>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="101" t="s">
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="81" t="s">
         <v>230</v>
       </c>
-      <c r="H20" s="99">
+      <c r="H20" s="79">
         <v>31</v>
       </c>
-      <c r="I20" s="100" t="s">
+      <c r="I20" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="J20" s="102" t="s">
+      <c r="J20" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="K20" s="99" t="s">
+      <c r="K20" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="L20" s="99" t="s">
+      <c r="L20" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="M20" s="99"/>
-      <c r="N20" s="99"/>
-      <c r="O20" s="102"/>
-      <c r="P20" s="100"/>
-      <c r="Q20" s="101">
+      <c r="M20" s="79"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="82"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="81">
         <v>7</v>
       </c>
-      <c r="R20" s="101" t="s">
+      <c r="R20" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="S20" s="101" t="s">
+      <c r="S20" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="T20" s="101" t="s">
+      <c r="T20" s="81" t="s">
         <v>230</v>
       </c>
-      <c r="U20" s="101" t="s">
+      <c r="U20" s="81" t="s">
         <v>231</v>
       </c>
       <c r="V20" s="30"/>
@@ -3199,46 +3202,46 @@
       <c r="C21" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="99" t="s">
+      <c r="D21" s="79" t="s">
         <v>233</v>
       </c>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="101" t="s">
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="81" t="s">
         <v>230</v>
       </c>
-      <c r="H21" s="99">
+      <c r="H21" s="79">
         <v>32</v>
       </c>
-      <c r="I21" s="100" t="s">
+      <c r="I21" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="J21" s="102" t="s">
+      <c r="J21" s="82" t="s">
         <v>236</v>
       </c>
-      <c r="K21" s="99" t="s">
+      <c r="K21" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="L21" s="99" t="s">
+      <c r="L21" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="M21" s="99"/>
-      <c r="N21" s="99"/>
-      <c r="O21" s="102"/>
-      <c r="P21" s="100"/>
-      <c r="Q21" s="101">
+      <c r="M21" s="79"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="82"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="81">
         <v>7</v>
       </c>
-      <c r="R21" s="101" t="s">
+      <c r="R21" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="S21" s="101" t="s">
+      <c r="S21" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="T21" s="101" t="s">
-        <v>230</v>
-      </c>
-      <c r="U21" s="101" t="s">
+      <c r="T21" s="81" t="s">
+        <v>237</v>
+      </c>
+      <c r="U21" s="81" t="s">
         <v>231</v>
       </c>
       <c r="V21" s="30"/>
@@ -3269,46 +3272,46 @@
       <c r="C22" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="99" t="s">
+      <c r="D22" s="79" t="s">
         <v>233</v>
       </c>
-      <c r="E22" s="100" t="s">
+      <c r="E22" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="100"/>
-      <c r="G22" s="101" t="s">
+      <c r="F22" s="80"/>
+      <c r="G22" s="81" t="s">
         <v>234</v>
       </c>
-      <c r="H22" s="99">
+      <c r="H22" s="79">
         <v>33</v>
       </c>
-      <c r="I22" s="100" t="s">
+      <c r="I22" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="J22" s="102"/>
-      <c r="K22" s="99" t="s">
+      <c r="J22" s="82"/>
+      <c r="K22" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="L22" s="99" t="s">
+      <c r="L22" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="M22" s="99"/>
-      <c r="N22" s="99"/>
-      <c r="O22" s="102"/>
-      <c r="P22" s="100"/>
-      <c r="Q22" s="101">
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="81">
         <v>7</v>
       </c>
-      <c r="R22" s="101" t="s">
+      <c r="R22" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="S22" s="101" t="s">
+      <c r="S22" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="T22" s="101" t="s">
+      <c r="T22" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="U22" s="101" t="s">
+      <c r="U22" s="81" t="s">
         <v>231</v>
       </c>
       <c r="V22" s="30"/>
@@ -5370,12 +5373,6 @@
     <row r="1090" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -5390,6 +5387,12 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K40">

</xml_diff>